<commit_message>
ürün excel impot düzenleme
</commit_message>
<xml_diff>
--- a/Infoline.WorkOfTime/Infoline.WorkOfTime.WebProject/Content/SampleExcels/product_template.xlsx
+++ b/Infoline.WorkOfTime/Infoline.WorkOfTime.WebProject/Content/SampleExcels/product_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr codeName="BuÇalışmaKitabı" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Infoline\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmet.undemir\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95128699-1786-4FAB-A48C-1A043B95C634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C25B8F-0465-4FB6-8851-2AA12418E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7DFFFC23-4D83-40A3-843B-3652B55E7F1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7DFFFC23-4D83-40A3-843B-3652B55E7F1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ürün - Stok" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
   <si>
     <t>Telefon</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Hizmet</t>
   </si>
   <si>
-    <t>Mamül(Ticari Mal)</t>
-  </si>
-  <si>
     <t>Yarı Mamül</t>
   </si>
   <si>
@@ -243,22 +240,31 @@
     <t>Çok Fonksiyonlu Yazıcı</t>
   </si>
   <si>
-    <t>Kodu *</t>
-  </si>
-  <si>
-    <t>İsmi *</t>
-  </si>
-  <si>
-    <t>Birimi *</t>
-  </si>
-  <si>
-    <t>Türü *</t>
-  </si>
-  <si>
-    <t>Stok Takip Tipi *</t>
-  </si>
-  <si>
-    <t>Barkod Tipi *</t>
+    <t>Mamül (Ticari Mal)</t>
+  </si>
+  <si>
+    <t>Kodu</t>
+  </si>
+  <si>
+    <t>İsmi</t>
+  </si>
+  <si>
+    <t>Birimi</t>
+  </si>
+  <si>
+    <t>Türü</t>
+  </si>
+  <si>
+    <t>Stok Takip Tipi</t>
+  </si>
+  <si>
+    <t>Barkod Tipi</t>
+  </si>
+  <si>
+    <t>Sütun1</t>
+  </si>
+  <si>
+    <t>Sütun2</t>
   </si>
 </sst>
 </file>
@@ -314,7 +320,10 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -323,10 +332,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -353,18 +359,20 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B91C2810-FB38-4B35-9A9D-5833510B1896}" name="AdayOgrenci" displayName="AdayOgrenci" ref="A1:K1048576" totalsRowShown="0">
   <autoFilter ref="A1:K1048576" xr:uid="{359CC720-9E8E-40E4-BCFC-DDD50204509D}"/>
-  <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{17AAE868-FACB-4914-83A8-01948ACDBCA3}" name="Kodu *" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{C0982E4C-1D7E-4E3B-8FE3-990CE4D847D0}" name="İsmi *" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{15956F2B-BA3C-458F-B107-26A411F11616}" name="Birimi *"/>
-    <tableColumn id="9" xr3:uid="{D187B37F-7B77-472A-9349-577E564C8554}" name="Türü *"/>
-    <tableColumn id="10" xr3:uid="{F34609F9-E99F-424E-89DC-D6843F7A3D4A}" name="Stok Takip Tipi *"/>
-    <tableColumn id="11" xr3:uid="{B04148F6-4AAB-47DB-802B-33F2EB7C4D52}" name="Barkod Tipi *" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{BE71FEE3-ED8D-43D3-BC01-70AE4F0D8506}" name="Birim Maaliyet (Vergiler Hariç)" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{304811C5-8F44-4699-B731-B895D8AB19C5}" name="Birim Satış Fiyatı (Vergiler Hariç)" dataDxfId="0"/>
-    <tableColumn id="15" xr3:uid="{0C4E74E4-5AA9-4593-B6B0-544EE2557786}" name="Marka" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{77C619D0-F9DA-4BDE-9B89-CEAF62A3EF45}" name="Kategori" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{65D56211-CCF1-40D8-BEEF-CA38A8D18962}" name="Açıklama" dataDxfId="4"/>
+  <tableColumns count="13">
+    <tableColumn id="6" xr3:uid="{17AAE868-FACB-4914-83A8-01948ACDBCA3}" name="Kodu" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{C0982E4C-1D7E-4E3B-8FE3-990CE4D847D0}" name="İsmi" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{15956F2B-BA3C-458F-B107-26A411F11616}" name="Birimi"/>
+    <tableColumn id="9" xr3:uid="{D187B37F-7B77-472A-9349-577E564C8554}" name="Türü"/>
+    <tableColumn id="2" xr3:uid="{D5CF88EF-49BD-413F-AD23-C5F913365DBF}" name="Stok Takip Tipi"/>
+    <tableColumn id="4" xr3:uid="{9C5CD844-591B-4FE9-82C8-ED1F556986CC}" name="Barkod Tipi"/>
+    <tableColumn id="10" xr3:uid="{F34609F9-E99F-424E-89DC-D6843F7A3D4A}" name="Birim Maaliyet (Vergiler Hariç)"/>
+    <tableColumn id="11" xr3:uid="{B04148F6-4AAB-47DB-802B-33F2EB7C4D52}" name="Birim Satış Fiyatı (Vergiler Hariç)" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{BE71FEE3-ED8D-43D3-BC01-70AE4F0D8506}" name="Marka" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{304811C5-8F44-4699-B731-B895D8AB19C5}" name="Kategori" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{0C4E74E4-5AA9-4593-B6B0-544EE2557786}" name="Açıklama" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{77C619D0-F9DA-4BDE-9B89-CEAF62A3EF45}" name="Sütun1" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{65D56211-CCF1-40D8-BEEF-CA38A8D18962}" name="Sütun2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -670,22 +678,22 @@
   <sheetPr codeName="Sayfa1"/>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="32" style="4" customWidth="1"/>
     <col min="9" max="11" width="32" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
@@ -705,22 +713,22 @@
         <v>73</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -734,10 +742,10 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" s="4">
         <v>960.5</v>
@@ -746,16 +754,16 @@
         <v>1450</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -766,13 +774,13 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G3" s="4">
         <v>4500</v>
@@ -781,16 +789,16 @@
         <v>5550.6</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -801,13 +809,13 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G4" s="4">
         <v>3450</v>
@@ -816,16 +824,16 @@
         <v>5900</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
     </row>
   </sheetData>
@@ -837,7 +845,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="1006" yWindow="313" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Uyarı!" error="Listeden seçim yapınız." prompt="Lütfen listeden seçim yapınız" xr:uid="{5C6C3FEA-CB23-4CD7-96F1-9717CC634568}">
           <x14:formula1>
             <xm:f>Birim!$A:$A</xm:f>
@@ -876,112 +884,112 @@
       <selection sqref="A1:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
     </row>
   </sheetData>
@@ -994,37 +1002,37 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1040,24 +1048,24 @@
       <selection sqref="A1:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1074,107 +1082,107 @@
       <selection sqref="A1:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>

</xml_diff>